<commit_message>
export option added (and others)
</commit_message>
<xml_diff>
--- a/data_sets/event_data.xlsx
+++ b/data_sets/event_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuel/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manu/metrics/data_sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCE40B6B-E9B7-2245-9529-76F9CCAA0ED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A2862-6254-4645-A8E9-DA622534D77E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendees" sheetId="1" r:id="rId1"/>
@@ -3093,7 +3093,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:N33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>